<commit_message>
Paper modifications and result checks
</commit_message>
<xml_diff>
--- a/RSA_2019_08/X6_Data/KLDivUttWorkers_x6_UttChoiceSimpleRSA_2019_06_03new.xlsx
+++ b/RSA_2019_08/X6_Data/KLDivUttWorkers_x6_UttChoiceSimpleRSA_2019_06_03new.xlsx
@@ -1052,8 +1052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H67" sqref="H67"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64:A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3624,150 +3624,150 @@
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A61" s="4">
-        <v>7</v>
-      </c>
-      <c r="B61" s="5">
-        <v>2.9038721366574101</v>
-      </c>
-      <c r="C61" s="5">
-        <v>0.238961018894427</v>
-      </c>
-      <c r="D61" s="5">
-        <v>0.239987780605322</v>
-      </c>
-      <c r="E61" s="5">
-        <v>2.7223378505428402</v>
-      </c>
-      <c r="F61" s="5"/>
-      <c r="G61" s="5">
-        <f t="shared" ref="G61:G68" si="7">B61-C61</f>
-        <v>2.664911117762983</v>
-      </c>
-      <c r="H61" s="5">
-        <f t="shared" ref="H61:H68" si="8">B61-D61</f>
-        <v>2.6638843560520882</v>
-      </c>
-      <c r="I61" s="5">
-        <f t="shared" ref="I61:I68" si="9">B61-E61</f>
-        <v>0.1815342861145699</v>
-      </c>
-      <c r="J61" s="5"/>
-      <c r="K61" s="5">
-        <v>-0.243637829895227</v>
-      </c>
-      <c r="L61" s="5">
-        <v>3.1541086086981601E-3</v>
-      </c>
-      <c r="M61" s="5">
-        <v>-2.5816379481700999</v>
-      </c>
-      <c r="N61" s="5">
-        <v>0</v>
-      </c>
-      <c r="O61" s="5">
-        <v>4.6371057760572598E-2</v>
-      </c>
-      <c r="P61" s="6">
-        <v>0.81059909765927596</v>
+      <c r="A61" s="7">
+        <v>41</v>
+      </c>
+      <c r="B61" s="8">
+        <v>1.0716912994708601</v>
+      </c>
+      <c r="C61" s="8">
+        <v>0.77838824703420795</v>
+      </c>
+      <c r="D61" s="8">
+        <v>0.74913561135821904</v>
+      </c>
+      <c r="E61" s="8">
+        <v>0.522106936979435</v>
+      </c>
+      <c r="F61" s="8"/>
+      <c r="G61" s="8">
+        <f>B61-C61</f>
+        <v>0.29330305243665211</v>
+      </c>
+      <c r="H61" s="8">
+        <f>B61-D61</f>
+        <v>0.32255568811264101</v>
+      </c>
+      <c r="I61" s="8">
+        <f>B61-E61</f>
+        <v>0.54958436249142506</v>
+      </c>
+      <c r="J61" s="8"/>
+      <c r="K61" s="8">
+        <v>-5.45816258858354E-2</v>
+      </c>
+      <c r="L61" s="8">
+        <v>0.468229185971481</v>
+      </c>
+      <c r="M61" s="8">
+        <v>-10</v>
+      </c>
+      <c r="N61" s="8">
+        <v>7.9544732174244802E-4</v>
+      </c>
+      <c r="O61" s="8">
+        <v>0.53206043689617499</v>
+      </c>
+      <c r="P61" s="9">
+        <v>-5.4824206590580902</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A62" s="7">
-        <v>0</v>
-      </c>
-      <c r="B62" s="8">
-        <v>3.6404247596124999</v>
-      </c>
-      <c r="C62" s="8">
-        <v>0.98867145977168103</v>
-      </c>
-      <c r="D62" s="8">
-        <v>0.96601259723578703</v>
-      </c>
-      <c r="E62" s="8">
-        <v>3.4493534141140798</v>
-      </c>
-      <c r="F62" s="8"/>
-      <c r="G62" s="8">
-        <f t="shared" si="7"/>
-        <v>2.6517532998408191</v>
-      </c>
-      <c r="H62" s="8">
-        <f t="shared" si="8"/>
-        <v>2.6744121623767128</v>
-      </c>
-      <c r="I62" s="8">
-        <f t="shared" si="9"/>
-        <v>0.19107134549842009</v>
-      </c>
-      <c r="J62" s="8"/>
-      <c r="K62" s="8">
-        <v>-0.24036888837337</v>
-      </c>
-      <c r="L62" s="8">
-        <v>8.9225908022692396E-2</v>
-      </c>
-      <c r="M62" s="8">
+      <c r="A62" s="4">
+        <v>11</v>
+      </c>
+      <c r="B62" s="5">
+        <v>1.1799060422627601</v>
+      </c>
+      <c r="C62" s="5">
+        <v>0.72450290035323905</v>
+      </c>
+      <c r="D62" s="5">
+        <v>0.70956472200660203</v>
+      </c>
+      <c r="E62" s="5">
+        <v>0.53105447314459797</v>
+      </c>
+      <c r="F62" s="5"/>
+      <c r="G62" s="5">
+        <f>B62-C62</f>
+        <v>0.45540314190952103</v>
+      </c>
+      <c r="H62" s="5">
+        <f>B62-D62</f>
+        <v>0.47034132025615805</v>
+      </c>
+      <c r="I62" s="5">
+        <f>B62-E62</f>
+        <v>0.64885156911816211</v>
+      </c>
+      <c r="J62" s="5"/>
+      <c r="K62" s="5">
+        <v>-6.6946519972340704E-2</v>
+      </c>
+      <c r="L62" s="5">
+        <v>0.38991795407688201</v>
+      </c>
+      <c r="M62" s="5">
         <v>-10</v>
       </c>
-      <c r="N62" s="8">
-        <v>0</v>
-      </c>
-      <c r="O62" s="8">
-        <v>5.0454498413993201E-2</v>
-      </c>
-      <c r="P62" s="9">
-        <v>1.14708043634274</v>
+      <c r="N62" s="5">
+        <v>6.8746661326015996E-4</v>
+      </c>
+      <c r="O62" s="5">
+        <v>0.40990482459231897</v>
+      </c>
+      <c r="P62" s="6">
+        <v>-5.0925935410044501</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="7">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="B63" s="8">
-        <v>2.04446066663006</v>
+        <v>1.64168833514449</v>
       </c>
       <c r="C63" s="8">
-        <v>0.27659435684581302</v>
+        <v>0.82985350763402899</v>
       </c>
       <c r="D63" s="8">
-        <v>0.24276920584335401</v>
+        <v>0.81490540983669002</v>
       </c>
       <c r="E63" s="8">
-        <v>0.242769205838331</v>
+        <v>0.82985350414120596</v>
       </c>
       <c r="F63" s="8"/>
       <c r="G63" s="8">
-        <f t="shared" si="7"/>
-        <v>1.7678663097842469</v>
+        <f>B63-C63</f>
+        <v>0.81183482751046099</v>
       </c>
       <c r="H63" s="8">
-        <f t="shared" si="8"/>
-        <v>1.8016914607867061</v>
+        <f>B63-D63</f>
+        <v>0.82678292530779995</v>
       </c>
       <c r="I63" s="8">
-        <f t="shared" si="9"/>
-        <v>1.8016914607917289</v>
+        <f>B63-E63</f>
+        <v>0.81183483100328402</v>
       </c>
       <c r="J63" s="8"/>
       <c r="K63" s="8">
-        <v>-0.16187921293251201</v>
+        <v>-9.0069128527877296E-2</v>
       </c>
       <c r="L63" s="8">
-        <v>0.15069951153729499</v>
+        <v>0.28018142834107301</v>
       </c>
       <c r="M63" s="8">
-        <v>-10</v>
+        <v>-9.7404672183631806</v>
       </c>
       <c r="N63" s="8">
-        <v>0.15069948498226701</v>
+        <v>0</v>
       </c>
       <c r="O63" s="8">
         <v>0</v>
       </c>
       <c r="P63" s="9">
-        <v>-10</v>
+        <v>-9.0063364077812902E-2</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
@@ -3788,15 +3788,15 @@
       </c>
       <c r="F64" s="5"/>
       <c r="G64" s="5">
-        <f t="shared" si="7"/>
+        <f>B64-C64</f>
         <v>1.3057217474003302</v>
       </c>
       <c r="H64" s="5">
-        <f t="shared" si="8"/>
+        <f>B64-D64</f>
         <v>1.3499047317533499</v>
       </c>
       <c r="I64" s="5">
-        <f t="shared" si="9"/>
+        <f>B64-E64</f>
         <v>1.3499047317899606</v>
       </c>
       <c r="J64" s="5"/>
@@ -3837,15 +3837,15 @@
       </c>
       <c r="F65" s="8"/>
       <c r="G65" s="8">
-        <f t="shared" si="7"/>
+        <f>B65-C65</f>
         <v>1.30704352855525</v>
       </c>
       <c r="H65" s="8">
-        <f t="shared" si="8"/>
+        <f>B65-D65</f>
         <v>1.3237264982907531</v>
       </c>
       <c r="I65" s="8">
-        <f t="shared" si="9"/>
+        <f>B65-E65</f>
         <v>0.85110176753040001</v>
       </c>
       <c r="J65" s="8"/>
@@ -3870,149 +3870,149 @@
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="7">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="B66" s="8">
-        <v>1.64168833514449</v>
+        <v>2.04446066663006</v>
       </c>
       <c r="C66" s="8">
-        <v>0.82985350763402899</v>
+        <v>0.27659435684581302</v>
       </c>
       <c r="D66" s="8">
-        <v>0.81490540983669002</v>
+        <v>0.24276920584335401</v>
       </c>
       <c r="E66" s="8">
-        <v>0.82985350414120596</v>
+        <v>0.242769205838331</v>
       </c>
       <c r="F66" s="8"/>
       <c r="G66" s="8">
-        <f t="shared" si="7"/>
-        <v>0.81183482751046099</v>
+        <f>B66-C66</f>
+        <v>1.7678663097842469</v>
       </c>
       <c r="H66" s="8">
-        <f t="shared" si="8"/>
-        <v>0.82678292530779995</v>
+        <f>B66-D66</f>
+        <v>1.8016914607867061</v>
       </c>
       <c r="I66" s="8">
-        <f t="shared" si="9"/>
-        <v>0.81183483100328402</v>
+        <f>B66-E66</f>
+        <v>1.8016914607917289</v>
       </c>
       <c r="J66" s="8"/>
       <c r="K66" s="8">
-        <v>-9.0069128527877296E-2</v>
+        <v>-0.16187921293251201</v>
       </c>
       <c r="L66" s="8">
-        <v>0.28018142834107301</v>
+        <v>0.15069951153729499</v>
       </c>
       <c r="M66" s="8">
-        <v>-9.7404672183631806</v>
+        <v>-10</v>
       </c>
       <c r="N66" s="8">
-        <v>0</v>
+        <v>0.15069948498226701</v>
       </c>
       <c r="O66" s="8">
         <v>0</v>
       </c>
       <c r="P66" s="9">
-        <v>-9.0063364077812902E-2</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A67" s="4">
-        <v>11</v>
-      </c>
-      <c r="B67" s="5">
-        <v>1.1799060422627601</v>
-      </c>
-      <c r="C67" s="5">
-        <v>0.72450290035323905</v>
-      </c>
-      <c r="D67" s="5">
-        <v>0.70956472200660203</v>
-      </c>
-      <c r="E67" s="5">
-        <v>0.53105447314459797</v>
-      </c>
-      <c r="F67" s="5"/>
-      <c r="G67" s="5">
-        <f t="shared" si="7"/>
-        <v>0.45540314190952103</v>
-      </c>
-      <c r="H67" s="5">
-        <f t="shared" si="8"/>
-        <v>0.47034132025615805</v>
-      </c>
-      <c r="I67" s="5">
-        <f t="shared" si="9"/>
-        <v>0.64885156911816211</v>
-      </c>
-      <c r="J67" s="5"/>
-      <c r="K67" s="5">
-        <v>-6.6946519972340704E-2</v>
-      </c>
-      <c r="L67" s="5">
-        <v>0.38991795407688201</v>
-      </c>
-      <c r="M67" s="5">
+      <c r="A67" s="7">
+        <v>0</v>
+      </c>
+      <c r="B67" s="8">
+        <v>3.6404247596124999</v>
+      </c>
+      <c r="C67" s="8">
+        <v>0.98867145977168103</v>
+      </c>
+      <c r="D67" s="8">
+        <v>0.96601259723578703</v>
+      </c>
+      <c r="E67" s="8">
+        <v>3.4493534141140798</v>
+      </c>
+      <c r="F67" s="8"/>
+      <c r="G67" s="8">
+        <f>B67-C67</f>
+        <v>2.6517532998408191</v>
+      </c>
+      <c r="H67" s="8">
+        <f>B67-D67</f>
+        <v>2.6744121623767128</v>
+      </c>
+      <c r="I67" s="8">
+        <f>B67-E67</f>
+        <v>0.19107134549842009</v>
+      </c>
+      <c r="J67" s="8"/>
+      <c r="K67" s="8">
+        <v>-0.24036888837337</v>
+      </c>
+      <c r="L67" s="8">
+        <v>8.9225908022692396E-2</v>
+      </c>
+      <c r="M67" s="8">
         <v>-10</v>
       </c>
-      <c r="N67" s="5">
-        <v>6.8746661326015996E-4</v>
-      </c>
-      <c r="O67" s="5">
-        <v>0.40990482459231897</v>
-      </c>
-      <c r="P67" s="6">
-        <v>-5.0925935410044501</v>
+      <c r="N67" s="8">
+        <v>0</v>
+      </c>
+      <c r="O67" s="8">
+        <v>5.0454498413993201E-2</v>
+      </c>
+      <c r="P67" s="9">
+        <v>1.14708043634274</v>
       </c>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A68" s="7">
-        <v>41</v>
-      </c>
-      <c r="B68" s="8">
-        <v>1.0716912994708601</v>
-      </c>
-      <c r="C68" s="8">
-        <v>0.77838824703420795</v>
-      </c>
-      <c r="D68" s="8">
-        <v>0.74913561135821904</v>
-      </c>
-      <c r="E68" s="8">
-        <v>0.522106936979435</v>
-      </c>
-      <c r="F68" s="8"/>
-      <c r="G68" s="8">
-        <f t="shared" si="7"/>
-        <v>0.29330305243665211</v>
-      </c>
-      <c r="H68" s="8">
-        <f t="shared" si="8"/>
-        <v>0.32255568811264101</v>
-      </c>
-      <c r="I68" s="8">
-        <f t="shared" si="9"/>
-        <v>0.54958436249142506</v>
-      </c>
-      <c r="J68" s="8"/>
-      <c r="K68" s="8">
-        <v>-5.45816258858354E-2</v>
-      </c>
-      <c r="L68" s="8">
-        <v>0.468229185971481</v>
-      </c>
-      <c r="M68" s="8">
-        <v>-10</v>
-      </c>
-      <c r="N68" s="8">
-        <v>7.9544732174244802E-4</v>
-      </c>
-      <c r="O68" s="8">
-        <v>0.53206043689617499</v>
-      </c>
-      <c r="P68" s="9">
-        <v>-5.4824206590580902</v>
+      <c r="A68" s="4">
+        <v>7</v>
+      </c>
+      <c r="B68" s="5">
+        <v>2.9038721366574101</v>
+      </c>
+      <c r="C68" s="5">
+        <v>0.238961018894427</v>
+      </c>
+      <c r="D68" s="5">
+        <v>0.239987780605322</v>
+      </c>
+      <c r="E68" s="5">
+        <v>2.7223378505428402</v>
+      </c>
+      <c r="F68" s="5"/>
+      <c r="G68" s="5">
+        <f>B68-C68</f>
+        <v>2.664911117762983</v>
+      </c>
+      <c r="H68" s="5">
+        <f>B68-D68</f>
+        <v>2.6638843560520882</v>
+      </c>
+      <c r="I68" s="5">
+        <f>B68-E68</f>
+        <v>0.1815342861145699</v>
+      </c>
+      <c r="J68" s="5"/>
+      <c r="K68" s="5">
+        <v>-0.243637829895227</v>
+      </c>
+      <c r="L68" s="5">
+        <v>3.1541086086981601E-3</v>
+      </c>
+      <c r="M68" s="5">
+        <v>-2.5816379481700999</v>
+      </c>
+      <c r="N68" s="5">
+        <v>0</v>
+      </c>
+      <c r="O68" s="5">
+        <v>4.6371057760572598E-2</v>
+      </c>
+      <c r="P68" s="6">
+        <v>0.81059909765927596</v>
       </c>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.25">
@@ -4042,29 +4042,29 @@
         <v>25.311116674902049</v>
       </c>
       <c r="C70" s="11">
-        <f t="shared" ref="C70:I70" si="10">SUM(C61:C68)</f>
-        <v>14.053279649701786</v>
+        <f t="shared" ref="C70:I70" si="7">SUM(C61:C68)</f>
+        <v>14.053279649701787</v>
       </c>
       <c r="D70" s="11">
-        <f t="shared" si="10"/>
-        <v>13.877817531965842</v>
+        <f t="shared" si="7"/>
+        <v>13.877817531965841</v>
       </c>
       <c r="E70" s="11">
-        <f t="shared" si="10"/>
-        <v>18.925542320564094</v>
+        <f t="shared" si="7"/>
+        <v>18.925542320564098</v>
       </c>
       <c r="F70" s="11"/>
       <c r="G70" s="11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>11.257837025200264</v>
       </c>
       <c r="H70" s="11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>11.43329914293621</v>
       </c>
       <c r="I70" s="11">
-        <f t="shared" si="10"/>
-        <v>6.3855743543379502</v>
+        <f t="shared" si="7"/>
+        <v>6.3855743543379511</v>
       </c>
       <c r="J70" s="11"/>
       <c r="K70" s="11"/>
@@ -4169,15 +4169,15 @@
       </c>
       <c r="F76" s="8"/>
       <c r="G76" s="8">
-        <f t="shared" ref="G76:G108" si="11">B76-C76</f>
+        <f>B76-C76</f>
         <v>3.421221288803955E-3</v>
       </c>
       <c r="H76" s="8">
-        <f t="shared" ref="H76:H108" si="12">B76-D76</f>
+        <f>B76-D76</f>
         <v>2.1849736204562986E-2</v>
       </c>
       <c r="I76" s="8">
-        <f t="shared" ref="I76:I108" si="13">B76-E76</f>
+        <f>B76-E76</f>
         <v>3.2492286659787983E-2</v>
       </c>
       <c r="J76" s="8"/>
@@ -4202,149 +4202,149 @@
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B77" s="5">
-        <v>4.40234625154807</v>
+        <v>0.16557467605741999</v>
       </c>
       <c r="C77" s="5">
-        <v>4.3233444946318196</v>
+        <v>0.160082050204159</v>
       </c>
       <c r="D77" s="5">
-        <v>4.3262945231005796</v>
+        <v>0.105477856604639</v>
       </c>
       <c r="E77" s="5">
-        <v>4.3261317692492796</v>
+        <v>0.10547785660452</v>
       </c>
       <c r="F77" s="5"/>
       <c r="G77" s="5">
-        <f t="shared" si="11"/>
-        <v>7.9001756916250443E-2</v>
+        <f>B77-C77</f>
+        <v>5.4926258532609906E-3</v>
       </c>
       <c r="H77" s="5">
-        <f t="shared" si="12"/>
-        <v>7.6051728447490419E-2</v>
+        <f>B77-D77</f>
+        <v>6.0096819452780989E-2</v>
       </c>
       <c r="I77" s="5">
-        <f t="shared" si="13"/>
-        <v>7.6214482298790465E-2</v>
+        <f>B77-E77</f>
+        <v>6.0096819452899991E-2</v>
       </c>
       <c r="J77" s="5"/>
       <c r="K77" s="5">
+        <v>2.4300253947209999E-2</v>
+      </c>
+      <c r="L77" s="5">
+        <v>0.95108160678990605</v>
+      </c>
+      <c r="M77" s="5">
+        <v>10</v>
+      </c>
+      <c r="N77" s="5">
+        <v>0.95108133060470201</v>
+      </c>
+      <c r="O77" s="5">
+        <v>0</v>
+      </c>
+      <c r="P77" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A78" s="7">
+        <v>23</v>
+      </c>
+      <c r="B78" s="8">
+        <v>0.25702748400186598</v>
+      </c>
+      <c r="C78" s="8">
+        <v>0.18614039356717799</v>
+      </c>
+      <c r="D78" s="8">
+        <v>0.118029261539282</v>
+      </c>
+      <c r="E78" s="8">
+        <v>0.118029261539289</v>
+      </c>
+      <c r="F78" s="8"/>
+      <c r="G78" s="8">
+        <f>B78-C78</f>
+        <v>7.0887090434687994E-2</v>
+      </c>
+      <c r="H78" s="8">
+        <f>B78-D78</f>
+        <v>0.13899822246258398</v>
+      </c>
+      <c r="I78" s="8">
+        <f>B78-E78</f>
+        <v>0.13899822246257698</v>
+      </c>
+      <c r="J78" s="8"/>
+      <c r="K78" s="8">
+        <v>3.2756247853725703E-2</v>
+      </c>
+      <c r="L78" s="8">
+        <v>0.72962597956348496</v>
+      </c>
+      <c r="M78" s="8">
+        <v>10</v>
+      </c>
+      <c r="N78" s="8">
+        <v>0.72962598392662004</v>
+      </c>
+      <c r="O78" s="8">
+        <v>0</v>
+      </c>
+      <c r="P78" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A79" s="4">
+        <v>10</v>
+      </c>
+      <c r="B79" s="5">
+        <v>4.40234625154807</v>
+      </c>
+      <c r="C79" s="5">
+        <v>4.3233444946318196</v>
+      </c>
+      <c r="D79" s="5">
+        <v>4.3262945231005796</v>
+      </c>
+      <c r="E79" s="5">
+        <v>4.3261317692492796</v>
+      </c>
+      <c r="F79" s="5"/>
+      <c r="G79" s="5">
+        <f>B79-C79</f>
+        <v>7.9001756916250443E-2</v>
+      </c>
+      <c r="H79" s="5">
+        <f>B79-D79</f>
+        <v>7.6051728447490419E-2</v>
+      </c>
+      <c r="I79" s="5">
+        <f>B79-E79</f>
+        <v>7.6214482298790465E-2</v>
+      </c>
+      <c r="J79" s="5"/>
+      <c r="K79" s="5">
         <v>2.3996784100335799E-2</v>
       </c>
-      <c r="L77" s="5">
+      <c r="L79" s="5">
         <v>4.7400023986126196E-3</v>
       </c>
-      <c r="M77" s="5">
+      <c r="M79" s="5">
         <v>0.27836781172719599</v>
       </c>
-      <c r="N77" s="5">
+      <c r="N79" s="5">
         <v>3.30855315307493E-3</v>
       </c>
-      <c r="O77" s="5">
-        <v>0</v>
-      </c>
-      <c r="P77" s="6">
+      <c r="O79" s="5">
+        <v>0</v>
+      </c>
+      <c r="P79" s="6">
         <v>0.25462851941880799</v>
-      </c>
-    </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A78" s="4">
-        <v>16</v>
-      </c>
-      <c r="B78" s="5">
-        <v>0.16557467605741999</v>
-      </c>
-      <c r="C78" s="5">
-        <v>0.160082050204159</v>
-      </c>
-      <c r="D78" s="5">
-        <v>0.105477856604639</v>
-      </c>
-      <c r="E78" s="5">
-        <v>0.10547785660452</v>
-      </c>
-      <c r="F78" s="5"/>
-      <c r="G78" s="5">
-        <f t="shared" si="11"/>
-        <v>5.4926258532609906E-3</v>
-      </c>
-      <c r="H78" s="5">
-        <f t="shared" si="12"/>
-        <v>6.0096819452780989E-2</v>
-      </c>
-      <c r="I78" s="5">
-        <f t="shared" si="13"/>
-        <v>6.0096819452899991E-2</v>
-      </c>
-      <c r="J78" s="5"/>
-      <c r="K78" s="5">
-        <v>2.4300253947209999E-2</v>
-      </c>
-      <c r="L78" s="5">
-        <v>0.95108160678990605</v>
-      </c>
-      <c r="M78" s="5">
-        <v>10</v>
-      </c>
-      <c r="N78" s="5">
-        <v>0.95108133060470201</v>
-      </c>
-      <c r="O78" s="5">
-        <v>0</v>
-      </c>
-      <c r="P78" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A79" s="7">
-        <v>23</v>
-      </c>
-      <c r="B79" s="8">
-        <v>0.25702748400186598</v>
-      </c>
-      <c r="C79" s="8">
-        <v>0.18614039356717799</v>
-      </c>
-      <c r="D79" s="8">
-        <v>0.118029261539282</v>
-      </c>
-      <c r="E79" s="8">
-        <v>0.118029261539289</v>
-      </c>
-      <c r="F79" s="8"/>
-      <c r="G79" s="8">
-        <f t="shared" si="11"/>
-        <v>7.0887090434687994E-2</v>
-      </c>
-      <c r="H79" s="8">
-        <f t="shared" si="12"/>
-        <v>0.13899822246258398</v>
-      </c>
-      <c r="I79" s="8">
-        <f t="shared" si="13"/>
-        <v>0.13899822246257698</v>
-      </c>
-      <c r="J79" s="8"/>
-      <c r="K79" s="8">
-        <v>3.2756247853725703E-2</v>
-      </c>
-      <c r="L79" s="8">
-        <v>0.72962597956348496</v>
-      </c>
-      <c r="M79" s="8">
-        <v>10</v>
-      </c>
-      <c r="N79" s="8">
-        <v>0.72962598392662004</v>
-      </c>
-      <c r="O79" s="8">
-        <v>0</v>
-      </c>
-      <c r="P79" s="9">
-        <v>10</v>
       </c>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.25">
@@ -4365,15 +4365,15 @@
       </c>
       <c r="F80" s="8"/>
       <c r="G80" s="8">
-        <f t="shared" si="11"/>
+        <f>B80-C80</f>
         <v>0.10820994272730022</v>
       </c>
       <c r="H80" s="8">
-        <f t="shared" si="12"/>
+        <f>B80-D80</f>
         <v>0.12196128553065</v>
       </c>
       <c r="I80" s="8">
-        <f t="shared" si="13"/>
+        <f>B80-E80</f>
         <v>0.19183223957758022</v>
       </c>
       <c r="J80" s="8"/>
@@ -4414,15 +4414,15 @@
       </c>
       <c r="F81" s="5"/>
       <c r="G81" s="5">
-        <f t="shared" si="11"/>
+        <f>B81-C81</f>
         <v>0.13883611887535299</v>
       </c>
       <c r="H81" s="5">
-        <f t="shared" si="12"/>
+        <f>B81-D81</f>
         <v>0.18734573361076098</v>
       </c>
       <c r="I81" s="5">
-        <f t="shared" si="13"/>
+        <f>B81-E81</f>
         <v>0.187345733610774</v>
       </c>
       <c r="J81" s="5"/>
@@ -4447,51 +4447,51 @@
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" s="7">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="B82" s="8">
-        <v>7.0493166566224099</v>
+        <v>7.42298540802269</v>
       </c>
       <c r="C82" s="8">
-        <v>6.4764487628394001</v>
+        <v>7.2425130600803804</v>
       </c>
       <c r="D82" s="8">
-        <v>6.4863110356531397</v>
+        <v>7.04321824654044</v>
       </c>
       <c r="E82" s="8">
-        <v>6.4864423932450102</v>
+        <v>7.0432182465368198</v>
       </c>
       <c r="F82" s="8"/>
       <c r="G82" s="8">
-        <f t="shared" si="11"/>
-        <v>0.57286789378300984</v>
+        <f>B82-C82</f>
+        <v>0.1804723479423096</v>
       </c>
       <c r="H82" s="8">
-        <f t="shared" si="12"/>
-        <v>0.5630056209692702</v>
+        <f>B82-D82</f>
+        <v>0.37976716148224998</v>
       </c>
       <c r="I82" s="8">
-        <f t="shared" si="13"/>
-        <v>0.56287426337739976</v>
+        <f>B82-E82</f>
+        <v>0.3797671614858702</v>
       </c>
       <c r="J82" s="8"/>
       <c r="K82" s="8">
-        <v>4.3606595167936503E-2</v>
+        <v>5.75520565511531E-2</v>
       </c>
       <c r="L82" s="8">
-        <v>2.43063454764199E-3</v>
+        <v>0.48295294520694498</v>
       </c>
       <c r="M82" s="8">
-        <v>0.42837533747356499</v>
+        <v>10</v>
       </c>
       <c r="N82" s="8">
-        <v>2.44510604665759E-3</v>
+        <v>0.482952630709447</v>
       </c>
       <c r="O82" s="8">
         <v>0</v>
       </c>
       <c r="P82" s="9">
-        <v>0.43677431297240599</v>
+        <v>10</v>
       </c>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.25">
@@ -4512,15 +4512,15 @@
       </c>
       <c r="F83" s="5"/>
       <c r="G83" s="5">
-        <f t="shared" si="11"/>
+        <f>B83-C83</f>
         <v>0.22853773217496998</v>
       </c>
       <c r="H83" s="5">
-        <f t="shared" si="12"/>
+        <f>B83-D83</f>
         <v>0.34709983353831997</v>
       </c>
       <c r="I83" s="5">
-        <f t="shared" si="13"/>
+        <f>B83-E83</f>
         <v>0.34709983353813989</v>
       </c>
       <c r="J83" s="5"/>
@@ -4544,394 +4544,394 @@
       </c>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A84" s="7">
+      <c r="A84" s="4">
+        <v>28</v>
+      </c>
+      <c r="B84" s="5">
+        <v>5.3785911828932296</v>
+      </c>
+      <c r="C84" s="5">
+        <v>5.0532646694374597</v>
+      </c>
+      <c r="D84" s="5">
+        <v>4.8908391061984897</v>
+      </c>
+      <c r="E84" s="5">
+        <v>4.94794054659378</v>
+      </c>
+      <c r="F84" s="5"/>
+      <c r="G84" s="5">
+        <f>B84-C84</f>
+        <v>0.32532651345576991</v>
+      </c>
+      <c r="H84" s="5">
+        <f>B84-D84</f>
+        <v>0.48775207669473986</v>
+      </c>
+      <c r="I84" s="5">
+        <f>B84-E84</f>
+        <v>0.43065063629944955</v>
+      </c>
+      <c r="J84" s="5"/>
+      <c r="K84" s="5">
+        <v>5.6927447467184901E-2</v>
+      </c>
+      <c r="L84" s="5">
+        <v>0.45950314576272</v>
+      </c>
+      <c r="M84" s="5">
+        <v>10</v>
+      </c>
+      <c r="N84" s="5">
+        <v>6.4995788278409403E-4</v>
+      </c>
+      <c r="O84" s="5">
+        <v>1.20829247118351E-2</v>
+      </c>
+      <c r="P84" s="6">
+        <v>1.26569923262367</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A85" s="7">
+        <v>8</v>
+      </c>
+      <c r="B85" s="8">
+        <v>7.4347458396014803</v>
+      </c>
+      <c r="C85" s="8">
+        <v>7.0165403882578801</v>
+      </c>
+      <c r="D85" s="8">
+        <v>6.8736800449111</v>
+      </c>
+      <c r="E85" s="8">
+        <v>6.8736800449062798</v>
+      </c>
+      <c r="F85" s="8"/>
+      <c r="G85" s="8">
+        <f>B85-C85</f>
+        <v>0.41820545134360021</v>
+      </c>
+      <c r="H85" s="8">
+        <f>B85-D85</f>
+        <v>0.56106579469038032</v>
+      </c>
+      <c r="I85" s="8">
+        <f>B85-E85</f>
+        <v>0.56106579469520046</v>
+      </c>
+      <c r="J85" s="8"/>
+      <c r="K85" s="8">
+        <v>5.8722769884339603E-2</v>
+      </c>
+      <c r="L85" s="8">
+        <v>0.44055426705404199</v>
+      </c>
+      <c r="M85" s="8">
+        <v>10</v>
+      </c>
+      <c r="N85" s="8">
+        <v>0.44055400902153802</v>
+      </c>
+      <c r="O85" s="8">
+        <v>0</v>
+      </c>
+      <c r="P85" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A86" s="7">
         <v>6</v>
       </c>
-      <c r="B84" s="8">
+      <c r="B86" s="8">
         <v>6.4454933360290099</v>
       </c>
-      <c r="C84" s="8">
+      <c r="C86" s="8">
         <v>5.9529233344633301</v>
       </c>
-      <c r="D84" s="8">
+      <c r="D86" s="8">
         <v>5.9572788720203098</v>
       </c>
-      <c r="E84" s="8">
+      <c r="E86" s="8">
         <v>5.9583360959207097</v>
       </c>
-      <c r="F84" s="8"/>
-      <c r="G84" s="8">
-        <f t="shared" si="11"/>
+      <c r="F86" s="8"/>
+      <c r="G86" s="8">
+        <f>B86-C86</f>
         <v>0.49257000156567976</v>
       </c>
-      <c r="H84" s="8">
-        <f t="shared" si="12"/>
+      <c r="H86" s="8">
+        <f>B86-D86</f>
         <v>0.48821446400870006</v>
       </c>
-      <c r="I84" s="8">
-        <f t="shared" si="13"/>
+      <c r="I86" s="8">
+        <f>B86-E86</f>
         <v>0.48715724010830019</v>
       </c>
-      <c r="J84" s="8"/>
-      <c r="K84" s="8">
+      <c r="J86" s="8"/>
+      <c r="K86" s="8">
         <v>5.3054998363894199E-2</v>
       </c>
-      <c r="L84" s="8">
+      <c r="L86" s="8">
         <v>2.5189194380160801E-3</v>
       </c>
-      <c r="M84" s="8">
+      <c r="M86" s="8">
         <v>0.52705472949129695</v>
       </c>
-      <c r="N84" s="8">
+      <c r="N86" s="8">
         <v>5.7459272419194598E-3</v>
       </c>
-      <c r="O84" s="8">
-        <v>0</v>
-      </c>
-      <c r="P84" s="9">
+      <c r="O86" s="8">
+        <v>0</v>
+      </c>
+      <c r="P86" s="9">
         <v>0.65613594815352805</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A85" s="4">
-        <v>49</v>
-      </c>
-      <c r="B85" s="5">
-        <v>5.4328929401399897</v>
-      </c>
-      <c r="C85" s="5">
-        <v>4.6549876981354101</v>
-      </c>
-      <c r="D85" s="5">
-        <v>4.6651128929933501</v>
-      </c>
-      <c r="E85" s="5">
-        <v>4.6681860188640698</v>
-      </c>
-      <c r="F85" s="5"/>
-      <c r="G85" s="5">
-        <f t="shared" si="11"/>
-        <v>0.77790524200457956</v>
-      </c>
-      <c r="H85" s="5">
-        <f t="shared" si="12"/>
-        <v>0.76778004714663961</v>
-      </c>
-      <c r="I85" s="5">
-        <f t="shared" si="13"/>
-        <v>0.76470692127591988</v>
-      </c>
-      <c r="J85" s="5"/>
-      <c r="K85" s="5">
-        <v>5.5396774000468697E-2</v>
-      </c>
-      <c r="L85" s="5">
-        <v>3.0022204319784499E-3</v>
-      </c>
-      <c r="M85" s="5">
-        <v>0.573553202402865</v>
-      </c>
-      <c r="N85" s="5">
-        <v>8.0287096299046495E-4</v>
-      </c>
-      <c r="O85" s="5">
-        <v>1.8292982162279502E-2</v>
-      </c>
-      <c r="P85" s="6">
-        <v>1.00966777026036</v>
-      </c>
-    </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A86" s="4">
-        <v>28</v>
-      </c>
-      <c r="B86" s="5">
-        <v>5.3785911828932296</v>
-      </c>
-      <c r="C86" s="5">
-        <v>5.0532646694374597</v>
-      </c>
-      <c r="D86" s="5">
-        <v>4.8908391061984897</v>
-      </c>
-      <c r="E86" s="5">
-        <v>4.94794054659378</v>
-      </c>
-      <c r="F86" s="5"/>
-      <c r="G86" s="5">
-        <f t="shared" si="11"/>
-        <v>0.32532651345576991</v>
-      </c>
-      <c r="H86" s="5">
-        <f t="shared" si="12"/>
-        <v>0.48775207669473986</v>
-      </c>
-      <c r="I86" s="5">
-        <f t="shared" si="13"/>
-        <v>0.43065063629944955</v>
-      </c>
-      <c r="J86" s="5"/>
-      <c r="K86" s="5">
-        <v>5.6927447467184901E-2</v>
-      </c>
-      <c r="L86" s="5">
-        <v>0.45950314576272</v>
-      </c>
-      <c r="M86" s="5">
-        <v>10</v>
-      </c>
-      <c r="N86" s="5">
-        <v>6.4995788278409403E-4</v>
-      </c>
-      <c r="O86" s="5">
-        <v>1.20829247118351E-2</v>
-      </c>
-      <c r="P86" s="6">
-        <v>1.26569923262367</v>
-      </c>
-    </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A87" s="7">
-        <v>52</v>
-      </c>
-      <c r="B87" s="8">
-        <v>7.42298540802269</v>
-      </c>
-      <c r="C87" s="8">
-        <v>7.2425130600803804</v>
-      </c>
-      <c r="D87" s="8">
-        <v>7.04321824654044</v>
-      </c>
-      <c r="E87" s="8">
-        <v>7.0432182465368198</v>
-      </c>
-      <c r="F87" s="8"/>
-      <c r="G87" s="8">
-        <f t="shared" si="11"/>
-        <v>0.1804723479423096</v>
-      </c>
-      <c r="H87" s="8">
-        <f t="shared" si="12"/>
-        <v>0.37976716148224998</v>
-      </c>
-      <c r="I87" s="8">
-        <f t="shared" si="13"/>
-        <v>0.3797671614858702</v>
-      </c>
-      <c r="J87" s="8"/>
-      <c r="K87" s="8">
-        <v>5.75520565511531E-2</v>
-      </c>
-      <c r="L87" s="8">
-        <v>0.48295294520694498</v>
-      </c>
-      <c r="M87" s="8">
-        <v>10</v>
-      </c>
-      <c r="N87" s="8">
-        <v>0.482952630709447</v>
-      </c>
-      <c r="O87" s="8">
-        <v>0</v>
-      </c>
-      <c r="P87" s="9">
+      <c r="A87" s="4">
+        <v>36</v>
+      </c>
+      <c r="B87" s="5">
+        <v>3.20441533378099</v>
+      </c>
+      <c r="C87" s="5">
+        <v>2.64089767626453</v>
+      </c>
+      <c r="D87" s="5">
+        <v>2.4882483271945599</v>
+      </c>
+      <c r="E87" s="5">
+        <v>2.48824832718751</v>
+      </c>
+      <c r="F87" s="5"/>
+      <c r="G87" s="5">
+        <f>B87-C87</f>
+        <v>0.56351765751645999</v>
+      </c>
+      <c r="H87" s="5">
+        <f>B87-D87</f>
+        <v>0.71616700658643007</v>
+      </c>
+      <c r="I87" s="5">
+        <f>B87-E87</f>
+        <v>0.71616700659347998</v>
+      </c>
+      <c r="J87" s="5"/>
+      <c r="K87" s="5">
+        <v>6.9439334888950099E-2</v>
+      </c>
+      <c r="L87" s="5">
+        <v>0.39252651023256002</v>
+      </c>
+      <c r="M87" s="5">
+        <v>10</v>
+      </c>
+      <c r="N87" s="5">
+        <v>0.39252629477145501</v>
+      </c>
+      <c r="O87" s="5">
+        <v>0</v>
+      </c>
+      <c r="P87" s="6">
         <v>10</v>
       </c>
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" s="7">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B88" s="8">
-        <v>7.4347458396014803</v>
+        <v>7.0493166566224099</v>
       </c>
       <c r="C88" s="8">
-        <v>7.0165403882578801</v>
+        <v>6.4764487628394001</v>
       </c>
       <c r="D88" s="8">
-        <v>6.8736800449111</v>
+        <v>6.4863110356531397</v>
       </c>
       <c r="E88" s="8">
-        <v>6.8736800449062798</v>
+        <v>6.4864423932450102</v>
       </c>
       <c r="F88" s="8"/>
       <c r="G88" s="8">
-        <f t="shared" si="11"/>
-        <v>0.41820545134360021</v>
+        <f>B88-C88</f>
+        <v>0.57286789378300984</v>
       </c>
       <c r="H88" s="8">
-        <f t="shared" si="12"/>
-        <v>0.56106579469038032</v>
+        <f>B88-D88</f>
+        <v>0.5630056209692702</v>
       </c>
       <c r="I88" s="8">
-        <f t="shared" si="13"/>
-        <v>0.56106579469520046</v>
+        <f>B88-E88</f>
+        <v>0.56287426337739976</v>
       </c>
       <c r="J88" s="8"/>
       <c r="K88" s="8">
-        <v>5.8722769884339603E-2</v>
+        <v>4.3606595167936503E-2</v>
       </c>
       <c r="L88" s="8">
-        <v>0.44055426705404199</v>
+        <v>2.43063454764199E-3</v>
       </c>
       <c r="M88" s="8">
-        <v>10</v>
+        <v>0.42837533747356499</v>
       </c>
       <c r="N88" s="8">
-        <v>0.44055400902153802</v>
+        <v>2.44510604665759E-3</v>
       </c>
       <c r="O88" s="8">
         <v>0</v>
       </c>
       <c r="P88" s="9">
-        <v>10</v>
+        <v>0.43677431297240599</v>
       </c>
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" s="4">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="B89" s="5">
-        <v>3.20441533378099</v>
+        <v>5.4328929401399897</v>
       </c>
       <c r="C89" s="5">
-        <v>2.64089767626453</v>
+        <v>4.6549876981354101</v>
       </c>
       <c r="D89" s="5">
-        <v>2.4882483271945599</v>
+        <v>4.6651128929933501</v>
       </c>
       <c r="E89" s="5">
-        <v>2.48824832718751</v>
+        <v>4.6681860188640698</v>
       </c>
       <c r="F89" s="5"/>
       <c r="G89" s="5">
-        <f t="shared" si="11"/>
-        <v>0.56351765751645999</v>
+        <f>B89-C89</f>
+        <v>0.77790524200457956</v>
       </c>
       <c r="H89" s="5">
-        <f t="shared" si="12"/>
-        <v>0.71616700658643007</v>
+        <f>B89-D89</f>
+        <v>0.76778004714663961</v>
       </c>
       <c r="I89" s="5">
-        <f t="shared" si="13"/>
-        <v>0.71616700659347998</v>
+        <f>B89-E89</f>
+        <v>0.76470692127591988</v>
       </c>
       <c r="J89" s="5"/>
       <c r="K89" s="5">
-        <v>6.9439334888950099E-2</v>
+        <v>5.5396774000468697E-2</v>
       </c>
       <c r="L89" s="5">
-        <v>0.39252651023256002</v>
+        <v>3.0022204319784499E-3</v>
       </c>
       <c r="M89" s="5">
-        <v>10</v>
+        <v>0.573553202402865</v>
       </c>
       <c r="N89" s="5">
-        <v>0.39252629477145501</v>
+        <v>8.0287096299046495E-4</v>
       </c>
       <c r="O89" s="5">
-        <v>0</v>
+        <v>1.8292982162279502E-2</v>
       </c>
       <c r="P89" s="6">
-        <v>10</v>
+        <v>1.00966777026036</v>
       </c>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A90" s="7">
+      <c r="A90" s="4">
+        <v>44</v>
+      </c>
+      <c r="B90" s="5">
+        <v>17.6536306307482</v>
+      </c>
+      <c r="C90" s="5">
+        <v>16.5654381403202</v>
+      </c>
+      <c r="D90" s="5">
+        <v>16.136675225641799</v>
+      </c>
+      <c r="E90" s="5">
+        <v>16.136675225542898</v>
+      </c>
+      <c r="F90" s="5"/>
+      <c r="G90" s="5">
+        <f>B90-C90</f>
+        <v>1.0881924904279998</v>
+      </c>
+      <c r="H90" s="5">
+        <f>B90-D90</f>
+        <v>1.5169554051064011</v>
+      </c>
+      <c r="I90" s="5">
+        <f>B90-E90</f>
+        <v>1.5169554052053016</v>
+      </c>
+      <c r="J90" s="5"/>
+      <c r="K90" s="5">
+        <v>9.5148254555016104E-2</v>
+      </c>
+      <c r="L90" s="5">
+        <v>0.287285192232002</v>
+      </c>
+      <c r="M90" s="5">
+        <v>10</v>
+      </c>
+      <c r="N90" s="5">
+        <v>0.287284177001639</v>
+      </c>
+      <c r="O90" s="5">
+        <v>0</v>
+      </c>
+      <c r="P90" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A91" s="7">
         <v>32</v>
       </c>
-      <c r="B90" s="8">
+      <c r="B91" s="8">
         <v>3.6040981012617501</v>
       </c>
-      <c r="C90" s="8">
+      <c r="C91" s="8">
         <v>2.37587171226295</v>
       </c>
-      <c r="D90" s="8">
+      <c r="D91" s="8">
         <v>2.18247855540345</v>
       </c>
-      <c r="E90" s="8">
+      <c r="E91" s="8">
         <v>2.18247855540262</v>
       </c>
-      <c r="F90" s="8"/>
-      <c r="G90" s="8">
-        <f t="shared" si="11"/>
+      <c r="F91" s="8"/>
+      <c r="G91" s="8">
+        <f>B91-C91</f>
         <v>1.2282263889988001</v>
       </c>
-      <c r="H90" s="8">
-        <f t="shared" si="12"/>
+      <c r="H91" s="8">
+        <f>B91-D91</f>
         <v>1.4216195458583001</v>
       </c>
-      <c r="I90" s="8">
-        <f t="shared" si="13"/>
+      <c r="I91" s="8">
+        <f>B91-E91</f>
         <v>1.4216195458591301</v>
       </c>
-      <c r="J90" s="8"/>
-      <c r="K90" s="8">
+      <c r="J91" s="8"/>
+      <c r="K91" s="8">
         <v>9.1026437780381206E-2</v>
       </c>
-      <c r="L90" s="8">
+      <c r="L91" s="8">
         <v>0.298508304007574</v>
       </c>
-      <c r="M90" s="8">
-        <v>10</v>
-      </c>
-      <c r="N90" s="8">
+      <c r="M91" s="8">
+        <v>10</v>
+      </c>
+      <c r="N91" s="8">
         <v>0.29850829577468901</v>
       </c>
-      <c r="O90" s="8">
-        <v>0</v>
-      </c>
-      <c r="P90" s="9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A91" s="4">
-        <v>44</v>
-      </c>
-      <c r="B91" s="5">
-        <v>17.6536306307482</v>
-      </c>
-      <c r="C91" s="5">
-        <v>16.5654381403202</v>
-      </c>
-      <c r="D91" s="5">
-        <v>16.136675225641799</v>
-      </c>
-      <c r="E91" s="5">
-        <v>16.136675225542898</v>
-      </c>
-      <c r="F91" s="5"/>
-      <c r="G91" s="5">
-        <f t="shared" si="11"/>
-        <v>1.0881924904279998</v>
-      </c>
-      <c r="H91" s="5">
-        <f t="shared" si="12"/>
-        <v>1.5169554051064011</v>
-      </c>
-      <c r="I91" s="5">
-        <f t="shared" si="13"/>
-        <v>1.5169554052053016</v>
-      </c>
-      <c r="J91" s="5"/>
-      <c r="K91" s="5">
-        <v>9.5148254555016104E-2</v>
-      </c>
-      <c r="L91" s="5">
-        <v>0.287285192232002</v>
-      </c>
-      <c r="M91" s="5">
-        <v>10</v>
-      </c>
-      <c r="N91" s="5">
-        <v>0.287284177001639</v>
-      </c>
-      <c r="O91" s="5">
-        <v>0</v>
-      </c>
-      <c r="P91" s="6">
+      <c r="O91" s="8">
+        <v>0</v>
+      </c>
+      <c r="P91" s="9">
         <v>10</v>
       </c>
     </row>
@@ -4953,15 +4953,15 @@
       </c>
       <c r="F92" s="5"/>
       <c r="G92" s="5">
-        <f t="shared" si="11"/>
+        <f>B92-C92</f>
         <v>1.3963358430118902</v>
       </c>
       <c r="H92" s="5">
-        <f t="shared" si="12"/>
+        <f>B92-D92</f>
         <v>1.7236101994838404</v>
       </c>
       <c r="I92" s="5">
-        <f t="shared" si="13"/>
+        <f>B92-E92</f>
         <v>1.7236101995095603</v>
       </c>
       <c r="J92" s="5"/>
@@ -5002,15 +5002,15 @@
       </c>
       <c r="F93" s="5"/>
       <c r="G93" s="5">
-        <f t="shared" si="11"/>
+        <f>B93-C93</f>
         <v>1.9919606802506706</v>
       </c>
       <c r="H93" s="5">
-        <f t="shared" si="12"/>
+        <f>B93-D93</f>
         <v>2.3717485966437106</v>
       </c>
       <c r="I93" s="5">
-        <f t="shared" si="13"/>
+        <f>B93-E93</f>
         <v>2.37174859626972</v>
       </c>
       <c r="J93" s="5"/>
@@ -5051,15 +5051,15 @@
       </c>
       <c r="F94" s="8"/>
       <c r="G94" s="8">
-        <f t="shared" si="11"/>
+        <f>B94-C94</f>
         <v>2.6932446650603694</v>
       </c>
       <c r="H94" s="8">
-        <f t="shared" si="12"/>
+        <f>B94-D94</f>
         <v>2.92662909347212</v>
       </c>
       <c r="I94" s="8">
-        <f t="shared" si="13"/>
+        <f>B94-E94</f>
         <v>2.7284856807969096</v>
       </c>
       <c r="J94" s="8"/>
@@ -5100,15 +5100,15 @@
       </c>
       <c r="F95" s="5"/>
       <c r="G95" s="5">
-        <f t="shared" si="11"/>
+        <f>B95-C95</f>
         <v>3.8008155157643104</v>
       </c>
       <c r="H95" s="5">
-        <f t="shared" si="12"/>
+        <f>B95-D95</f>
         <v>3.7840904443775303</v>
       </c>
       <c r="I95" s="5">
-        <f t="shared" si="13"/>
+        <f>B95-E95</f>
         <v>3.7847801688854501</v>
       </c>
       <c r="J95" s="5"/>
@@ -5149,15 +5149,15 @@
       </c>
       <c r="F96" s="8"/>
       <c r="G96" s="8">
-        <f t="shared" si="11"/>
+        <f>B96-C96</f>
         <v>4.522148706933601</v>
       </c>
       <c r="H96" s="8">
-        <f t="shared" si="12"/>
+        <f>B96-D96</f>
         <v>4.8848833419759004</v>
       </c>
       <c r="I96" s="8">
-        <f t="shared" si="13"/>
+        <f>B96-E96</f>
         <v>4.6033667617098004</v>
       </c>
       <c r="J96" s="8"/>
@@ -5182,149 +5182,149 @@
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" s="4">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="B97" s="5">
-        <v>18.517106716776599</v>
+        <v>8.7765432695636907</v>
       </c>
       <c r="C97" s="5">
-        <v>13.291192097413299</v>
+        <v>3.7126486770286502</v>
       </c>
       <c r="D97" s="5">
-        <v>12.6710600368946</v>
+        <v>3.25523449406636</v>
       </c>
       <c r="E97" s="5">
-        <v>13.099779724976999</v>
+        <v>3.2552344942329601</v>
       </c>
       <c r="F97" s="5"/>
       <c r="G97" s="5">
-        <f t="shared" si="11"/>
-        <v>5.2259146193632997</v>
+        <f>B97-C97</f>
+        <v>5.0638945925350409</v>
       </c>
       <c r="H97" s="5">
-        <f t="shared" si="12"/>
-        <v>5.846046679881999</v>
+        <f>B97-D97</f>
+        <v>5.5213087754973307</v>
       </c>
       <c r="I97" s="5">
-        <f t="shared" si="13"/>
-        <v>5.4173269917995999</v>
+        <f>B97-E97</f>
+        <v>5.5213087753307306</v>
       </c>
       <c r="J97" s="5"/>
       <c r="K97" s="5">
+        <v>0.19057462768019001</v>
+      </c>
+      <c r="L97" s="5">
+        <v>0.130959671085771</v>
+      </c>
+      <c r="M97" s="5">
+        <v>10</v>
+      </c>
+      <c r="N97" s="5">
+        <v>0.13095984273667499</v>
+      </c>
+      <c r="O97" s="5">
+        <v>0</v>
+      </c>
+      <c r="P97" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A98" s="7">
+        <v>9</v>
+      </c>
+      <c r="B98" s="8">
+        <v>11.003922079785999</v>
+      </c>
+      <c r="C98" s="8">
+        <v>5.8323530256999199</v>
+      </c>
+      <c r="D98" s="8">
+        <v>5.6665710706689998</v>
+      </c>
+      <c r="E98" s="8">
+        <v>5.7887977200734904</v>
+      </c>
+      <c r="F98" s="8"/>
+      <c r="G98" s="8">
+        <f>B98-C98</f>
+        <v>5.1715690540860795</v>
+      </c>
+      <c r="H98" s="8">
+        <f>B98-D98</f>
+        <v>5.3373510091169996</v>
+      </c>
+      <c r="I98" s="8">
+        <f>B98-E98</f>
+        <v>5.215124359712509</v>
+      </c>
+      <c r="J98" s="8"/>
+      <c r="K98" s="8">
+        <v>0.19319476654158699</v>
+      </c>
+      <c r="L98" s="8">
+        <v>0.13242612330282399</v>
+      </c>
+      <c r="M98" s="8">
+        <v>10</v>
+      </c>
+      <c r="N98" s="8">
+        <v>5.4690924102525499E-3</v>
+      </c>
+      <c r="O98" s="8">
+        <v>0</v>
+      </c>
+      <c r="P98" s="9">
+        <v>2.4116831370040601</v>
+      </c>
+    </row>
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A99" s="4">
+        <v>35</v>
+      </c>
+      <c r="B99" s="5">
+        <v>18.517106716776599</v>
+      </c>
+      <c r="C99" s="5">
+        <v>13.291192097413299</v>
+      </c>
+      <c r="D99" s="5">
+        <v>12.6710600368946</v>
+      </c>
+      <c r="E99" s="5">
+        <v>13.099779724976999</v>
+      </c>
+      <c r="F99" s="5"/>
+      <c r="G99" s="5">
+        <f>B99-C99</f>
+        <v>5.2259146193632997</v>
+      </c>
+      <c r="H99" s="5">
+        <f>B99-D99</f>
+        <v>5.846046679881999</v>
+      </c>
+      <c r="I99" s="5">
+        <f>B99-E99</f>
+        <v>5.4173269917995999</v>
+      </c>
+      <c r="J99" s="5"/>
+      <c r="K99" s="5">
         <v>0.189266165850381</v>
       </c>
-      <c r="L97" s="5">
+      <c r="L99" s="5">
         <v>0.12928454235254899</v>
       </c>
-      <c r="M97" s="5">
-        <v>10</v>
-      </c>
-      <c r="N97" s="5">
+      <c r="M99" s="5">
+        <v>10</v>
+      </c>
+      <c r="N99" s="5">
         <v>1.3765297415261001E-3</v>
       </c>
-      <c r="O97" s="5">
-        <v>0</v>
-      </c>
-      <c r="P97" s="6">
+      <c r="O99" s="5">
+        <v>0</v>
+      </c>
+      <c r="P99" s="6">
         <v>1.6198455028143399</v>
-      </c>
-    </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A98" s="4">
-        <v>5</v>
-      </c>
-      <c r="B98" s="5">
-        <v>8.7765432695636907</v>
-      </c>
-      <c r="C98" s="5">
-        <v>3.7126486770286502</v>
-      </c>
-      <c r="D98" s="5">
-        <v>3.25523449406636</v>
-      </c>
-      <c r="E98" s="5">
-        <v>3.2552344942329601</v>
-      </c>
-      <c r="F98" s="5"/>
-      <c r="G98" s="5">
-        <f t="shared" si="11"/>
-        <v>5.0638945925350409</v>
-      </c>
-      <c r="H98" s="5">
-        <f t="shared" si="12"/>
-        <v>5.5213087754973307</v>
-      </c>
-      <c r="I98" s="5">
-        <f t="shared" si="13"/>
-        <v>5.5213087753307306</v>
-      </c>
-      <c r="J98" s="5"/>
-      <c r="K98" s="5">
-        <v>0.19057462768019001</v>
-      </c>
-      <c r="L98" s="5">
-        <v>0.130959671085771</v>
-      </c>
-      <c r="M98" s="5">
-        <v>10</v>
-      </c>
-      <c r="N98" s="5">
-        <v>0.13095984273667499</v>
-      </c>
-      <c r="O98" s="5">
-        <v>0</v>
-      </c>
-      <c r="P98" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A99" s="7">
-        <v>9</v>
-      </c>
-      <c r="B99" s="8">
-        <v>11.003922079785999</v>
-      </c>
-      <c r="C99" s="8">
-        <v>5.8323530256999199</v>
-      </c>
-      <c r="D99" s="8">
-        <v>5.6665710706689998</v>
-      </c>
-      <c r="E99" s="8">
-        <v>5.7887977200734904</v>
-      </c>
-      <c r="F99" s="8"/>
-      <c r="G99" s="8">
-        <f t="shared" si="11"/>
-        <v>5.1715690540860795</v>
-      </c>
-      <c r="H99" s="8">
-        <f t="shared" si="12"/>
-        <v>5.3373510091169996</v>
-      </c>
-      <c r="I99" s="8">
-        <f t="shared" si="13"/>
-        <v>5.215124359712509</v>
-      </c>
-      <c r="J99" s="8"/>
-      <c r="K99" s="8">
-        <v>0.19319476654158699</v>
-      </c>
-      <c r="L99" s="8">
-        <v>0.13242612330282399</v>
-      </c>
-      <c r="M99" s="8">
-        <v>10</v>
-      </c>
-      <c r="N99" s="8">
-        <v>5.4690924102525499E-3</v>
-      </c>
-      <c r="O99" s="8">
-        <v>0</v>
-      </c>
-      <c r="P99" s="9">
-        <v>2.4116831370040601</v>
       </c>
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.25">
@@ -5345,15 +5345,15 @@
       </c>
       <c r="F100" s="8"/>
       <c r="G100" s="8">
-        <f t="shared" si="11"/>
+        <f>B100-C100</f>
         <v>5.7080876766900301</v>
       </c>
       <c r="H100" s="8">
-        <f t="shared" si="12"/>
+        <f>B100-D100</f>
         <v>6.3794652286931202</v>
       </c>
       <c r="I100" s="8">
-        <f t="shared" si="13"/>
+        <f>B100-E100</f>
         <v>5.8796859940783701</v>
       </c>
       <c r="J100" s="8"/>
@@ -5394,15 +5394,15 @@
       </c>
       <c r="F101" s="5"/>
       <c r="G101" s="5">
-        <f t="shared" si="11"/>
+        <f>B101-C101</f>
         <v>6.028329355483339</v>
       </c>
       <c r="H101" s="5">
-        <f t="shared" si="12"/>
+        <f>B101-D101</f>
         <v>6.3409959662688493</v>
       </c>
       <c r="I101" s="5">
-        <f t="shared" si="13"/>
+        <f>B101-E101</f>
         <v>6.0948067047561594</v>
       </c>
       <c r="J101" s="5"/>
@@ -5426,101 +5426,101 @@
       </c>
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A102" s="4">
+      <c r="A102" s="7">
+        <v>25</v>
+      </c>
+      <c r="B102" s="8">
+        <v>10.8845639397856</v>
+      </c>
+      <c r="C102" s="8">
+        <v>4.6124543077022704</v>
+      </c>
+      <c r="D102" s="8">
+        <v>4.0535109239430698</v>
+      </c>
+      <c r="E102" s="8">
+        <v>4.4812367657695802</v>
+      </c>
+      <c r="F102" s="8"/>
+      <c r="G102" s="8">
+        <f>B102-C102</f>
+        <v>6.2721096320833301</v>
+      </c>
+      <c r="H102" s="8">
+        <f>B102-D102</f>
+        <v>6.8310530158425307</v>
+      </c>
+      <c r="I102" s="8">
+        <f>B102-E102</f>
+        <v>6.4033271740160203</v>
+      </c>
+      <c r="J102" s="8"/>
+      <c r="K102" s="8">
+        <v>0.226575349439091</v>
+      </c>
+      <c r="L102" s="8">
+        <v>0.105171726244929</v>
+      </c>
+      <c r="M102" s="8">
+        <v>10</v>
+      </c>
+      <c r="N102" s="8">
+        <v>1.08776303565355E-3</v>
+      </c>
+      <c r="O102" s="8">
+        <v>0</v>
+      </c>
+      <c r="P102" s="9">
+        <v>1.7587501630401701</v>
+      </c>
+    </row>
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A103" s="4">
         <v>14</v>
       </c>
-      <c r="B102" s="5">
+      <c r="B103" s="5">
         <v>9.6894372167689102</v>
       </c>
-      <c r="C102" s="5">
+      <c r="C103" s="5">
         <v>3.3374106425684702</v>
       </c>
-      <c r="D102" s="5">
+      <c r="D103" s="5">
         <v>3.3748379562950901</v>
       </c>
-      <c r="E102" s="5">
+      <c r="E103" s="5">
         <v>3.3681705474447101</v>
       </c>
-      <c r="F102" s="5"/>
-      <c r="G102" s="5">
-        <f t="shared" si="11"/>
+      <c r="F103" s="5"/>
+      <c r="G103" s="5">
+        <f>B103-C103</f>
         <v>6.3520265742004405</v>
       </c>
-      <c r="H102" s="5">
-        <f t="shared" si="12"/>
+      <c r="H103" s="5">
+        <f>B103-D103</f>
         <v>6.3145992604738197</v>
       </c>
-      <c r="I102" s="5">
-        <f t="shared" si="13"/>
+      <c r="I103" s="5">
+        <f>B103-E103</f>
         <v>6.3212666693242001</v>
       </c>
-      <c r="J102" s="5"/>
-      <c r="K102" s="5">
+      <c r="J103" s="5"/>
+      <c r="K103" s="5">
         <v>0.21851466872734901</v>
       </c>
-      <c r="L102" s="5">
+      <c r="L103" s="5">
         <v>3.2224392588355599E-3</v>
       </c>
-      <c r="M102" s="5">
+      <c r="M103" s="5">
         <v>2.2969534364981001</v>
       </c>
-      <c r="N102" s="5">
+      <c r="N103" s="5">
         <v>1.4073999683964201E-3</v>
       </c>
-      <c r="O102" s="5">
-        <v>0</v>
-      </c>
-      <c r="P102" s="6">
+      <c r="O103" s="5">
+        <v>0</v>
+      </c>
+      <c r="P103" s="6">
         <v>1.91613896103244</v>
-      </c>
-    </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A103" s="7">
-        <v>25</v>
-      </c>
-      <c r="B103" s="8">
-        <v>10.8845639397856</v>
-      </c>
-      <c r="C103" s="8">
-        <v>4.6124543077022704</v>
-      </c>
-      <c r="D103" s="8">
-        <v>4.0535109239430698</v>
-      </c>
-      <c r="E103" s="8">
-        <v>4.4812367657695802</v>
-      </c>
-      <c r="F103" s="8"/>
-      <c r="G103" s="8">
-        <f t="shared" si="11"/>
-        <v>6.2721096320833301</v>
-      </c>
-      <c r="H103" s="8">
-        <f t="shared" si="12"/>
-        <v>6.8310530158425307</v>
-      </c>
-      <c r="I103" s="8">
-        <f t="shared" si="13"/>
-        <v>6.4033271740160203</v>
-      </c>
-      <c r="J103" s="8"/>
-      <c r="K103" s="8">
-        <v>0.226575349439091</v>
-      </c>
-      <c r="L103" s="8">
-        <v>0.105171726244929</v>
-      </c>
-      <c r="M103" s="8">
-        <v>10</v>
-      </c>
-      <c r="N103" s="8">
-        <v>1.08776303565355E-3</v>
-      </c>
-      <c r="O103" s="8">
-        <v>0</v>
-      </c>
-      <c r="P103" s="9">
-        <v>1.7587501630401701</v>
       </c>
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.25">
@@ -5541,15 +5541,15 @@
       </c>
       <c r="F104" s="8"/>
       <c r="G104" s="8">
-        <f t="shared" si="11"/>
+        <f>B104-C104</f>
         <v>7.1849352612373307</v>
       </c>
       <c r="H104" s="8">
-        <f t="shared" si="12"/>
+        <f>B104-D104</f>
         <v>7.6739678390946908</v>
       </c>
       <c r="I104" s="8">
-        <f t="shared" si="13"/>
+        <f>B104-E104</f>
         <v>7.312308747516461</v>
       </c>
       <c r="J104" s="8"/>
@@ -5590,15 +5590,15 @@
       </c>
       <c r="F105" s="5"/>
       <c r="G105" s="5">
-        <f t="shared" si="11"/>
+        <f>B105-C105</f>
         <v>7.2693080724557708</v>
       </c>
       <c r="H105" s="5">
-        <f t="shared" si="12"/>
+        <f>B105-D105</f>
         <v>7.7260657162584607</v>
       </c>
       <c r="I105" s="5">
-        <f t="shared" si="13"/>
+        <f>B105-E105</f>
         <v>7.3800419191032809</v>
       </c>
       <c r="J105" s="5"/>
@@ -5639,15 +5639,15 @@
       </c>
       <c r="F106" s="8"/>
       <c r="G106" s="8">
-        <f t="shared" si="11"/>
+        <f>B106-C106</f>
         <v>7.3391975915764096</v>
       </c>
       <c r="H106" s="8">
-        <f t="shared" si="12"/>
+        <f>B106-D106</f>
         <v>7.8124203908346903</v>
       </c>
       <c r="I106" s="8">
-        <f t="shared" si="13"/>
+        <f>B106-E106</f>
         <v>7.4552298922072797</v>
       </c>
       <c r="J106" s="8"/>
@@ -5688,15 +5688,15 @@
       </c>
       <c r="F107" s="5"/>
       <c r="G107" s="5">
-        <f t="shared" si="11"/>
+        <f>B107-C107</f>
         <v>8.5058347454876504</v>
       </c>
       <c r="H107" s="5">
-        <f t="shared" si="12"/>
+        <f>B107-D107</f>
         <v>8.6514191608207192</v>
       </c>
       <c r="I107" s="5">
-        <f t="shared" si="13"/>
+        <f>B107-E107</f>
         <v>8.2817784342627192</v>
       </c>
       <c r="J107" s="5"/>
@@ -5737,15 +5737,15 @@
       </c>
       <c r="F108" s="8"/>
       <c r="G108" s="8">
-        <f t="shared" si="11"/>
+        <f>B108-C108</f>
         <v>10.842714649547121</v>
       </c>
       <c r="H108" s="8">
-        <f t="shared" si="12"/>
+        <f>B108-D108</f>
         <v>10.958721108503822</v>
       </c>
       <c r="I108" s="8">
-        <f t="shared" si="13"/>
+        <f>B108-E108</f>
         <v>10.842714649649961</v>
       </c>
       <c r="J108" s="8"/>
@@ -5774,36 +5774,36 @@
       </c>
       <c r="B110">
         <f>SUM(B76:B108)</f>
-        <v>256.66447510510841</v>
+        <v>256.66447510510835</v>
       </c>
       <c r="C110">
-        <f t="shared" ref="C110:I110" si="14">SUM(C76:C108)</f>
+        <f t="shared" ref="C110:I110" si="8">SUM(C76:C108)</f>
         <v>155.01437739403283</v>
       </c>
       <c r="D110">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>147.72436879607798</v>
       </c>
       <c r="E110">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>151.45251979367902</v>
       </c>
       <c r="G110">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>101.6500977110755</v>
       </c>
       <c r="H110">
-        <f t="shared" si="14"/>
-        <v>108.9401063090304</v>
+        <f t="shared" si="8"/>
+        <v>108.94010630903038</v>
       </c>
       <c r="I110">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>105.21195531142935</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A58:P98">
-    <sortCondition ref="K58:K98"/>
+  <sortState ref="A61:P68">
+    <sortCondition ref="G61:G68"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>